<commit_message>
Update E8 HR Data - Calculations.xlsx
</commit_message>
<xml_diff>
--- a/Exercise Files/Exercise 8/E8 HR Data - Calculations.xlsx
+++ b/Exercise Files/Exercise 8/E8 HR Data - Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f21e54c367d3358c/Documents/01 Work Files/05 SSIT/Online Courses/Advanced PivotTables/Exercise Files/Exercise 8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wayvy Technologies\Documents\GitHub\PivotTables\Exercise Files\Exercise 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9D27A194-00BF-4D0A-9265-E015331961CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13F85008-1D1C-499B-9B16-350A3A888705}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F891E832-A7D4-4C0B-A0C9-BB6AD8A57265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Info" sheetId="1" r:id="rId1"/>
@@ -21,16 +21,17 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
     <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable11" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
     <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable21" hidden="1">'[1]Department Info'!$A$1:$A$100</definedName>
-    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31" hidden="1">'[1]Job Info'!$A$1:$A$100</definedName>
+    <definedName name="_xlcn.WorksheetConnection_HRDataConsolidating.xlsxTable31" hidden="1">'[2]Job Info'!$A$1:$A$100</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId7"/>
+    <pivotCache cacheId="12" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -578,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -587,10 +588,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -690,15 +690,26 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Department Info"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="Job Info"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1016,8 +1027,8 @@
         </groupItems>
       </fieldGroup>
     </cacheField>
-    <cacheField name="Bonus" numFmtId="0" formula="IF('Job Rating'=5,Salary*10%,0 )" databaseField="0"/>
-    <cacheField name="New Salary" numFmtId="0" formula="Salary+Bonus" databaseField="0"/>
+    <cacheField name="Bonus" numFmtId="0" formula="IF('Job Rating' =5,Salary *10%,0)" databaseField="0"/>
+    <cacheField name="New Salary" numFmtId="0" formula="Salary +Bonus" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -2122,7 +2133,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBF667DA-0437-474B-81FE-12A825857483}" name="PivotTable2" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBF667DA-0437-474B-81FE-12A825857483}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
   <location ref="A3:C103" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2648,7 +2659,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA7C68A1-D831-442D-85A5-C72BA69AA0B0}" name="PivotTable2" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA7C68A1-D831-442D-85A5-C72BA69AA0B0}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
   <location ref="A3:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -2908,7 +2919,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EEF074F-9D5B-4FFA-AB68-1D5FFB45081C}" name="PivotTable2" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4EEF074F-9D5B-4FFA-AB68-1D5FFB45081C}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
   <location ref="A3:E103" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -3442,7 +3453,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0C458C2C-B4AB-4134-A107-1260CBFF717A}" name="PivotTable2" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0C458C2C-B4AB-4134-A107-1260CBFF717A}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Department" customListSort="0">
   <location ref="A3:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -3720,9 +3731,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3760,7 +3771,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3866,7 +3877,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4008,7 +4019,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4022,19 +4033,19 @@
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="20.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4063,7 +4074,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2100</v>
       </c>
@@ -4092,7 +4103,7 @@
         <v>40445</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2101</v>
       </c>
@@ -4121,7 +4132,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2102</v>
       </c>
@@ -4150,7 +4161,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2103</v>
       </c>
@@ -4179,7 +4190,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2104</v>
       </c>
@@ -4208,7 +4219,7 @@
         <v>40164</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2105</v>
       </c>
@@ -4237,7 +4248,7 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2106</v>
       </c>
@@ -4266,7 +4277,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2107</v>
       </c>
@@ -4295,7 +4306,7 @@
         <v>38555</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2108</v>
       </c>
@@ -4324,7 +4335,7 @@
         <v>42421</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2109</v>
       </c>
@@ -4353,7 +4364,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2110</v>
       </c>
@@ -4382,7 +4393,7 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2111</v>
       </c>
@@ -4411,7 +4422,7 @@
         <v>40378</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2112</v>
       </c>
@@ -4440,7 +4451,7 @@
         <v>40976</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2113</v>
       </c>
@@ -4469,7 +4480,7 @@
         <v>36845</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2114</v>
       </c>
@@ -4498,7 +4509,7 @@
         <v>42217</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2115</v>
       </c>
@@ -4527,7 +4538,7 @@
         <v>41198</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2116</v>
       </c>
@@ -4556,7 +4567,7 @@
         <v>36704</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2117</v>
       </c>
@@ -4585,7 +4596,7 @@
         <v>42895</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2118</v>
       </c>
@@ -4614,7 +4625,7 @@
         <v>41286</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2119</v>
       </c>
@@ -4643,7 +4654,7 @@
         <v>39319</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2120</v>
       </c>
@@ -4672,7 +4683,7 @@
         <v>40839</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2121</v>
       </c>
@@ -4701,7 +4712,7 @@
         <v>36754</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2122</v>
       </c>
@@ -4730,7 +4741,7 @@
         <v>38170</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2123</v>
       </c>
@@ -4759,7 +4770,7 @@
         <v>39164</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2124</v>
       </c>
@@ -4788,7 +4799,7 @@
         <v>42219</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2125</v>
       </c>
@@ -4817,7 +4828,7 @@
         <v>40652</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2126</v>
       </c>
@@ -4846,7 +4857,7 @@
         <v>41065</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2127</v>
       </c>
@@ -4875,7 +4886,7 @@
         <v>39692</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2128</v>
       </c>
@@ -4904,7 +4915,7 @@
         <v>42030</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2129</v>
       </c>
@@ -4933,7 +4944,7 @@
         <v>39499</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2130</v>
       </c>
@@ -4962,7 +4973,7 @@
         <v>43695</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2131</v>
       </c>
@@ -4991,7 +5002,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2132</v>
       </c>
@@ -5020,7 +5031,7 @@
         <v>36600</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2133</v>
       </c>
@@ -5049,7 +5060,7 @@
         <v>39803</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2134</v>
       </c>
@@ -5078,7 +5089,7 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2135</v>
       </c>
@@ -5107,7 +5118,7 @@
         <v>38971</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2136</v>
       </c>
@@ -5136,7 +5147,7 @@
         <v>40276</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2137</v>
       </c>
@@ -5165,7 +5176,7 @@
         <v>38241</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2138</v>
       </c>
@@ -5194,7 +5205,7 @@
         <v>40684</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2139</v>
       </c>
@@ -5223,7 +5234,7 @@
         <v>39996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2140</v>
       </c>
@@ -5252,7 +5263,7 @@
         <v>37411</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2141</v>
       </c>
@@ -5281,7 +5292,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2142</v>
       </c>
@@ -5310,7 +5321,7 @@
         <v>43170</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2143</v>
       </c>
@@ -5339,7 +5350,7 @@
         <v>37292</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2144</v>
       </c>
@@ -5368,7 +5379,7 @@
         <v>37609</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2145</v>
       </c>
@@ -5397,7 +5408,7 @@
         <v>37094</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2146</v>
       </c>
@@ -5426,7 +5437,7 @@
         <v>42118</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2147</v>
       </c>
@@ -5455,7 +5466,7 @@
         <v>41517</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2148</v>
       </c>
@@ -5484,7 +5495,7 @@
         <v>38742</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2149</v>
       </c>
@@ -5513,7 +5524,7 @@
         <v>40047</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2150</v>
       </c>
@@ -5542,7 +5553,7 @@
         <v>39802</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2151</v>
       </c>
@@ -5571,7 +5582,7 @@
         <v>39616</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2152</v>
       </c>
@@ -5600,7 +5611,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2153</v>
       </c>
@@ -5629,7 +5640,7 @@
         <v>39019</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2154</v>
       </c>
@@ -5658,7 +5669,7 @@
         <v>41028</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2155</v>
       </c>
@@ -5687,7 +5698,7 @@
         <v>39768</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2156</v>
       </c>
@@ -5716,7 +5727,7 @@
         <v>41153</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2157</v>
       </c>
@@ -5745,7 +5756,7 @@
         <v>36847</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2158</v>
       </c>
@@ -5774,7 +5785,7 @@
         <v>37105</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2159</v>
       </c>
@@ -5803,7 +5814,7 @@
         <v>39744</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2160</v>
       </c>
@@ -5832,7 +5843,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2161</v>
       </c>
@@ -5861,7 +5872,7 @@
         <v>38401</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2162</v>
       </c>
@@ -5890,7 +5901,7 @@
         <v>37956</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2163</v>
       </c>
@@ -5919,7 +5930,7 @@
         <v>43907</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2164</v>
       </c>
@@ -5948,7 +5959,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2165</v>
       </c>
@@ -5977,7 +5988,7 @@
         <v>39740</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2166</v>
       </c>
@@ -6006,7 +6017,7 @@
         <v>40408</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2167</v>
       </c>
@@ -6035,7 +6046,7 @@
         <v>38822</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2168</v>
       </c>
@@ -6064,7 +6075,7 @@
         <v>40083</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2169</v>
       </c>
@@ -6093,7 +6104,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2170</v>
       </c>
@@ -6122,7 +6133,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2171</v>
       </c>
@@ -6151,7 +6162,7 @@
         <v>41582</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2172</v>
       </c>
@@ -6180,7 +6191,7 @@
         <v>36663</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2173</v>
       </c>
@@ -6209,7 +6220,7 @@
         <v>37526</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2174</v>
       </c>
@@ -6238,7 +6249,7 @@
         <v>41710</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2175</v>
       </c>
@@ -6267,7 +6278,7 @@
         <v>40274</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2176</v>
       </c>
@@ -6296,7 +6307,7 @@
         <v>40107</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2177</v>
       </c>
@@ -6325,7 +6336,7 @@
         <v>39142</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2178</v>
       </c>
@@ -6354,7 +6365,7 @@
         <v>39165</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2179</v>
       </c>
@@ -6383,7 +6394,7 @@
         <v>42462</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2180</v>
       </c>
@@ -6412,7 +6423,7 @@
         <v>41654</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2181</v>
       </c>
@@ -6441,7 +6452,7 @@
         <v>43128</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2182</v>
       </c>
@@ -6470,7 +6481,7 @@
         <v>43381</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2183</v>
       </c>
@@ -6499,7 +6510,7 @@
         <v>41676</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2184</v>
       </c>
@@ -6528,7 +6539,7 @@
         <v>36651</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2185</v>
       </c>
@@ -6557,7 +6568,7 @@
         <v>42526</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2186</v>
       </c>
@@ -6586,7 +6597,7 @@
         <v>38565</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2187</v>
       </c>
@@ -6615,7 +6626,7 @@
         <v>37518</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2188</v>
       </c>
@@ -6644,7 +6655,7 @@
         <v>39656</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2189</v>
       </c>
@@ -6673,7 +6684,7 @@
         <v>41701</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2190</v>
       </c>
@@ -6702,7 +6713,7 @@
         <v>42528</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2191</v>
       </c>
@@ -6731,7 +6742,7 @@
         <v>38499</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2192</v>
       </c>
@@ -6760,7 +6771,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2193</v>
       </c>
@@ -6789,7 +6800,7 @@
         <v>38384</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2194</v>
       </c>
@@ -6818,7 +6829,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2195</v>
       </c>
@@ -6847,7 +6858,7 @@
         <v>43124</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2196</v>
       </c>
@@ -6876,7 +6887,7 @@
         <v>37442</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2197</v>
       </c>
@@ -6905,7 +6916,7 @@
         <v>38690</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2198</v>
       </c>
@@ -6946,71 +6957,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20861FBA-D0EF-4462-8671-A8B3DD975D79}">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="35" max="40" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="47" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="68" max="72" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="79" max="80" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="91" max="93" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="96" max="104" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="40" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="47" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="72" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="93" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="104" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -7018,7 +7029,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>104</v>
       </c>
@@ -7029,1100 +7040,1100 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
       <c r="C4" s="5">
         <v>56146</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="5">
         <v>38206</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="5">
         <v>27714</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="5">
         <v>85983</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
       <c r="C8" s="5">
         <v>79270</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>5</v>
       </c>
       <c r="C9" s="5">
         <v>61939</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="8">
         <v>3</v>
       </c>
       <c r="C10" s="5">
         <v>94050</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="8">
         <v>1</v>
       </c>
       <c r="C11" s="5">
         <v>43304</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>3</v>
       </c>
       <c r="C12" s="5">
         <v>70085</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="8">
         <v>5</v>
       </c>
       <c r="C13" s="5">
         <v>99568</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="8">
         <v>1</v>
       </c>
       <c r="C14" s="5">
         <v>47852</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="8">
         <v>2</v>
       </c>
       <c r="C15" s="5">
         <v>71398</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="8">
         <v>3</v>
       </c>
       <c r="C16" s="5">
         <v>86734</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="8">
         <v>2</v>
       </c>
       <c r="C17" s="5">
         <v>52320</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="8">
         <v>4</v>
       </c>
       <c r="C18" s="5">
         <v>82871</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="8">
         <v>5</v>
       </c>
       <c r="C19" s="5">
         <v>67560</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="8">
         <v>5</v>
       </c>
       <c r="C20" s="5">
         <v>84859</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="8">
         <v>3</v>
       </c>
       <c r="C21" s="5">
         <v>99248</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="8">
         <v>5</v>
       </c>
       <c r="C22" s="5">
         <v>66314</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="8">
         <v>2</v>
       </c>
       <c r="C23" s="5">
         <v>37471</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="8">
         <v>4</v>
       </c>
       <c r="C24" s="5">
         <v>32172</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="8">
         <v>3</v>
       </c>
       <c r="C25" s="5">
         <v>92006</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="8">
         <v>2</v>
       </c>
       <c r="C26" s="5">
         <v>63016</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="8">
         <v>1</v>
       </c>
       <c r="C27" s="5">
         <v>74344</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="8">
         <v>2</v>
       </c>
       <c r="C28" s="5">
         <v>57759</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="8">
         <v>1</v>
       </c>
       <c r="C29" s="5">
         <v>50945</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="8">
         <v>1</v>
       </c>
       <c r="C30" s="5">
         <v>44737</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="8">
         <v>1</v>
       </c>
       <c r="C31" s="5">
         <v>71067</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="8">
         <v>2</v>
       </c>
       <c r="C32" s="5">
         <v>84304</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="8">
         <v>3</v>
       </c>
       <c r="C33" s="5">
         <v>90328</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="8">
         <v>3</v>
       </c>
       <c r="C34" s="5">
         <v>74903</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="8">
         <v>4</v>
       </c>
       <c r="C35" s="5">
         <v>32929</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="8">
         <v>1</v>
       </c>
       <c r="C36" s="5">
         <v>86135</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="8">
         <v>5</v>
       </c>
       <c r="C37" s="5">
         <v>50831</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="8">
         <v>3</v>
       </c>
       <c r="C38" s="5">
         <v>62997</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="8">
         <v>1</v>
       </c>
       <c r="C39" s="5">
         <v>27723</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="8">
         <v>1</v>
       </c>
       <c r="C40" s="5">
         <v>70918</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="8">
         <v>5</v>
       </c>
       <c r="C41" s="5">
         <v>95191</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="8">
         <v>5</v>
       </c>
       <c r="C42" s="5">
         <v>47939</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="8">
         <v>4</v>
       </c>
       <c r="C43" s="5">
         <v>47199</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="8">
         <v>4</v>
       </c>
       <c r="C44" s="5">
         <v>79980</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="8">
         <v>1</v>
       </c>
       <c r="C45" s="5">
         <v>55197</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="8">
         <v>5</v>
       </c>
       <c r="C46" s="5">
         <v>33900</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="8">
         <v>3</v>
       </c>
       <c r="C47" s="5">
         <v>72568</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="8">
         <v>5</v>
       </c>
       <c r="C48" s="5">
         <v>56102</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="8">
         <v>5</v>
       </c>
       <c r="C49" s="5">
         <v>63662</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="8">
         <v>2</v>
       </c>
       <c r="C50" s="5">
         <v>51651</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="8">
         <v>2</v>
       </c>
       <c r="C51" s="5">
         <v>85288</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="8">
         <v>1</v>
       </c>
       <c r="C52" s="5">
         <v>59404</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="8">
         <v>5</v>
       </c>
       <c r="C53" s="5">
         <v>87377</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="8">
         <v>1</v>
       </c>
       <c r="C54" s="5">
         <v>33787</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="8">
         <v>1</v>
       </c>
       <c r="C55" s="5">
         <v>29587</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="8">
         <v>2</v>
       </c>
       <c r="C56" s="5">
         <v>26402</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="8">
         <v>4</v>
       </c>
       <c r="C57" s="5">
         <v>74201</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="8">
         <v>5</v>
       </c>
       <c r="C58" s="5">
         <v>95346</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="8">
         <v>3</v>
       </c>
       <c r="C59" s="5">
         <v>33778</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="8">
         <v>1</v>
       </c>
       <c r="C60" s="5">
         <v>76212</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="8">
         <v>1</v>
       </c>
       <c r="C61" s="5">
         <v>96503</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="8">
         <v>1</v>
       </c>
       <c r="C62" s="5">
         <v>60066</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="8">
         <v>1</v>
       </c>
       <c r="C63" s="5">
         <v>79169</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="8">
         <v>1</v>
       </c>
       <c r="C64" s="5">
         <v>50558</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="8">
         <v>4</v>
       </c>
       <c r="C65" s="5">
         <v>50441</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="8">
         <v>1</v>
       </c>
       <c r="C66" s="5">
         <v>61955</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="8">
         <v>3</v>
       </c>
       <c r="C67" s="5">
         <v>52949</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="8">
         <v>3</v>
       </c>
       <c r="C68" s="5">
         <v>92526</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="8">
         <v>2</v>
       </c>
       <c r="C69" s="5">
         <v>83169</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="8">
         <v>2</v>
       </c>
       <c r="C70" s="5">
         <v>58190</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="8">
         <v>5</v>
       </c>
       <c r="C71" s="5">
         <v>91367</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="8">
         <v>5</v>
       </c>
       <c r="C72" s="5">
         <v>78694</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="8">
         <v>4</v>
       </c>
       <c r="C73" s="5">
         <v>53638</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="8">
         <v>3</v>
       </c>
       <c r="C74" s="5">
         <v>62472</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="8">
         <v>4</v>
       </c>
       <c r="C75" s="5">
         <v>89126</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="8">
         <v>4</v>
       </c>
       <c r="C76" s="5">
         <v>61590</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="8">
         <v>5</v>
       </c>
       <c r="C77" s="5">
         <v>86357</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="8">
         <v>2</v>
       </c>
       <c r="C78" s="5">
         <v>40979</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="8">
         <v>5</v>
       </c>
       <c r="C79" s="5">
         <v>90608</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="8">
         <v>4</v>
       </c>
       <c r="C80" s="5">
         <v>91632</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="8">
         <v>2</v>
       </c>
       <c r="C81" s="5">
         <v>38413</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="8">
         <v>4</v>
       </c>
       <c r="C82" s="5">
         <v>29892</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="8">
         <v>2</v>
       </c>
       <c r="C83" s="5">
         <v>85414</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="8">
         <v>3</v>
       </c>
       <c r="C84" s="5">
         <v>36220</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="8">
         <v>1</v>
       </c>
       <c r="C85" s="5">
         <v>54102</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="8">
         <v>2</v>
       </c>
       <c r="C86" s="5">
         <v>97719</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="8">
         <v>4</v>
       </c>
       <c r="C87" s="5">
         <v>83237</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="8">
         <v>1</v>
       </c>
       <c r="C88" s="5">
         <v>56934</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="8">
         <v>3</v>
       </c>
       <c r="C89" s="5">
         <v>78859</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="8">
         <v>2</v>
       </c>
       <c r="C90" s="5">
         <v>87369</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="8">
         <v>2</v>
       </c>
       <c r="C91" s="5">
         <v>25504</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="8">
         <v>4</v>
       </c>
       <c r="C92" s="5">
         <v>40689</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="8">
         <v>3</v>
       </c>
       <c r="C93" s="5">
         <v>78844</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="8">
         <v>2</v>
       </c>
       <c r="C94" s="5">
         <v>27077</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="8">
         <v>2</v>
       </c>
       <c r="C95" s="5">
         <v>51225</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="8">
         <v>1</v>
       </c>
       <c r="C96" s="5">
         <v>55175</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="8">
         <v>5</v>
       </c>
       <c r="C97" s="5">
         <v>87541</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="8">
         <v>4</v>
       </c>
       <c r="C98" s="5">
         <v>56445</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="8">
         <v>4</v>
       </c>
       <c r="C99" s="5">
         <v>64872</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="8">
         <v>1</v>
       </c>
       <c r="C100" s="5">
         <v>45587</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="8">
         <v>4</v>
       </c>
       <c r="C101" s="5">
         <v>48094</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="8">
         <v>5</v>
       </c>
       <c r="C102" s="5">
         <v>39748</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B103" s="8">
         <v>287</v>
       </c>
       <c r="C103" s="5">
@@ -8139,88 +8150,88 @@
   <dimension ref="A3:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" customWidth="1"/>
-    <col min="11" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="35" max="40" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="47" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="68" max="72" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="79" max="80" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="91" max="93" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="96" max="104" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="40" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="47" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="72" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="93" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="104" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>104</v>
       </c>
@@ -8233,151 +8244,151 @@
       <c r="D4" t="s">
         <v>125</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>9</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="8">
         <v>9</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="8">
         <v>18</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="8">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="8">
         <v>12</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="8">
         <v>9</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="8">
         <v>17</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="8">
         <v>13</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="8">
         <v>3</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="8">
         <v>12</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="8">
         <v>12</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="8">
         <v>6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="8">
         <v>18</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="8">
         <v>7</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="8">
         <v>2</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>62</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="8">
         <v>37</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="8">
         <v>99</v>
       </c>
     </row>
@@ -8393,70 +8404,71 @@
   </sheetPr>
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="35" max="40" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="47" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="68" max="72" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="79" max="80" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="91" max="93" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="96" max="104" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="40" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="47" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="72" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="93" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="104" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -8464,7 +8476,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>104</v>
       </c>
@@ -8481,11 +8493,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
       <c r="C4" s="5">
@@ -8498,11 +8510,11 @@
         <v>56146</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="5">
@@ -8515,11 +8527,11 @@
         <v>38206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="5">
@@ -8532,11 +8544,11 @@
         <v>27714</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="5">
@@ -8549,11 +8561,11 @@
         <v>94581.3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
       <c r="C8" s="5">
@@ -8566,11 +8578,11 @@
         <v>79270</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>5</v>
       </c>
       <c r="C9" s="5">
@@ -8583,11 +8595,11 @@
         <v>68132.899999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="8">
         <v>3</v>
       </c>
       <c r="C10" s="5">
@@ -8600,11 +8612,11 @@
         <v>94050</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="8">
         <v>1</v>
       </c>
       <c r="C11" s="5">
@@ -8617,11 +8629,11 @@
         <v>43304</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>3</v>
       </c>
       <c r="C12" s="5">
@@ -8634,11 +8646,11 @@
         <v>70085</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="8">
         <v>5</v>
       </c>
       <c r="C13" s="5">
@@ -8651,11 +8663,11 @@
         <v>109524.8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="8">
         <v>1</v>
       </c>
       <c r="C14" s="5">
@@ -8668,11 +8680,11 @@
         <v>47852</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="8">
         <v>2</v>
       </c>
       <c r="C15" s="5">
@@ -8685,11 +8697,11 @@
         <v>71398</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="8">
         <v>3</v>
       </c>
       <c r="C16" s="5">
@@ -8702,11 +8714,11 @@
         <v>86734</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="8">
         <v>2</v>
       </c>
       <c r="C17" s="5">
@@ -8719,11 +8731,11 @@
         <v>52320</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="8">
         <v>4</v>
       </c>
       <c r="C18" s="5">
@@ -8736,11 +8748,11 @@
         <v>82871</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="8">
         <v>5</v>
       </c>
       <c r="C19" s="5">
@@ -8753,11 +8765,11 @@
         <v>74316</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="8">
         <v>5</v>
       </c>
       <c r="C20" s="5">
@@ -8770,11 +8782,11 @@
         <v>93344.9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="8">
         <v>3</v>
       </c>
       <c r="C21" s="5">
@@ -8787,11 +8799,11 @@
         <v>99248</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="8">
         <v>5</v>
       </c>
       <c r="C22" s="5">
@@ -8804,11 +8816,11 @@
         <v>72945.399999999994</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="8">
         <v>2</v>
       </c>
       <c r="C23" s="5">
@@ -8821,11 +8833,11 @@
         <v>37471</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="8">
         <v>4</v>
       </c>
       <c r="C24" s="5">
@@ -8838,11 +8850,11 @@
         <v>32172</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="8">
         <v>3</v>
       </c>
       <c r="C25" s="5">
@@ -8855,11 +8867,11 @@
         <v>92006</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="8">
         <v>2</v>
       </c>
       <c r="C26" s="5">
@@ -8872,11 +8884,11 @@
         <v>63016</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="8">
         <v>1</v>
       </c>
       <c r="C27" s="5">
@@ -8889,11 +8901,11 @@
         <v>74344</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="8">
         <v>2</v>
       </c>
       <c r="C28" s="5">
@@ -8906,11 +8918,11 @@
         <v>57759</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="8">
         <v>1</v>
       </c>
       <c r="C29" s="5">
@@ -8923,11 +8935,11 @@
         <v>50945</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="8">
         <v>1</v>
       </c>
       <c r="C30" s="5">
@@ -8940,11 +8952,11 @@
         <v>44737</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="8">
         <v>1</v>
       </c>
       <c r="C31" s="5">
@@ -8957,11 +8969,11 @@
         <v>71067</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="8">
         <v>2</v>
       </c>
       <c r="C32" s="5">
@@ -8974,11 +8986,11 @@
         <v>84304</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="8">
         <v>3</v>
       </c>
       <c r="C33" s="5">
@@ -8991,11 +9003,11 @@
         <v>90328</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="8">
         <v>3</v>
       </c>
       <c r="C34" s="5">
@@ -9008,11 +9020,11 @@
         <v>74903</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="8">
         <v>4</v>
       </c>
       <c r="C35" s="5">
@@ -9025,11 +9037,11 @@
         <v>32929</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="8">
         <v>1</v>
       </c>
       <c r="C36" s="5">
@@ -9042,11 +9054,11 @@
         <v>86135</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="8">
         <v>5</v>
       </c>
       <c r="C37" s="5">
@@ -9059,11 +9071,11 @@
         <v>55914.1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="8">
         <v>3</v>
       </c>
       <c r="C38" s="5">
@@ -9076,11 +9088,11 @@
         <v>62997</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="8">
         <v>1</v>
       </c>
       <c r="C39" s="5">
@@ -9093,11 +9105,11 @@
         <v>27723</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="8">
         <v>1</v>
       </c>
       <c r="C40" s="5">
@@ -9110,11 +9122,11 @@
         <v>70918</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="8">
         <v>5</v>
       </c>
       <c r="C41" s="5">
@@ -9127,11 +9139,11 @@
         <v>104710.1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="8">
         <v>5</v>
       </c>
       <c r="C42" s="5">
@@ -9144,11 +9156,11 @@
         <v>52732.9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="8">
         <v>4</v>
       </c>
       <c r="C43" s="5">
@@ -9161,11 +9173,11 @@
         <v>47199</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="8">
         <v>4</v>
       </c>
       <c r="C44" s="5">
@@ -9178,11 +9190,11 @@
         <v>79980</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="8">
         <v>1</v>
       </c>
       <c r="C45" s="5">
@@ -9195,11 +9207,11 @@
         <v>55197</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="8">
         <v>5</v>
       </c>
       <c r="C46" s="5">
@@ -9212,11 +9224,11 @@
         <v>37290</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="8">
         <v>3</v>
       </c>
       <c r="C47" s="5">
@@ -9229,11 +9241,11 @@
         <v>72568</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="8">
         <v>5</v>
       </c>
       <c r="C48" s="5">
@@ -9246,11 +9258,11 @@
         <v>61712.2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="8">
         <v>5</v>
       </c>
       <c r="C49" s="5">
@@ -9263,11 +9275,11 @@
         <v>70028.2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="8">
         <v>2</v>
       </c>
       <c r="C50" s="5">
@@ -9280,11 +9292,11 @@
         <v>51651</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="8">
         <v>2</v>
       </c>
       <c r="C51" s="5">
@@ -9297,11 +9309,11 @@
         <v>85288</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="8">
         <v>1</v>
       </c>
       <c r="C52" s="5">
@@ -9314,11 +9326,11 @@
         <v>59404</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="8">
         <v>5</v>
       </c>
       <c r="C53" s="5">
@@ -9331,11 +9343,11 @@
         <v>96114.7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="8">
         <v>1</v>
       </c>
       <c r="C54" s="5">
@@ -9348,11 +9360,11 @@
         <v>33787</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="8">
         <v>1</v>
       </c>
       <c r="C55" s="5">
@@ -9365,11 +9377,11 @@
         <v>29587</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="8">
         <v>2</v>
       </c>
       <c r="C56" s="5">
@@ -9382,11 +9394,11 @@
         <v>26402</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="8">
         <v>4</v>
       </c>
       <c r="C57" s="5">
@@ -9399,11 +9411,11 @@
         <v>74201</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="8">
         <v>5</v>
       </c>
       <c r="C58" s="5">
@@ -9416,11 +9428,11 @@
         <v>104880.6</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="8">
         <v>3</v>
       </c>
       <c r="C59" s="5">
@@ -9433,11 +9445,11 @@
         <v>33778</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="8">
         <v>1</v>
       </c>
       <c r="C60" s="5">
@@ -9450,11 +9462,11 @@
         <v>76212</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="8">
         <v>1</v>
       </c>
       <c r="C61" s="5">
@@ -9467,11 +9479,11 @@
         <v>96503</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="8">
         <v>1</v>
       </c>
       <c r="C62" s="5">
@@ -9484,11 +9496,11 @@
         <v>60066</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="8">
         <v>1</v>
       </c>
       <c r="C63" s="5">
@@ -9501,11 +9513,11 @@
         <v>79169</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="8">
         <v>1</v>
       </c>
       <c r="C64" s="5">
@@ -9518,11 +9530,11 @@
         <v>50558</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="8">
         <v>4</v>
       </c>
       <c r="C65" s="5">
@@ -9535,11 +9547,11 @@
         <v>50441</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="8">
         <v>1</v>
       </c>
       <c r="C66" s="5">
@@ -9552,11 +9564,11 @@
         <v>61955</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="8">
         <v>3</v>
       </c>
       <c r="C67" s="5">
@@ -9569,11 +9581,11 @@
         <v>52949</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="8">
         <v>3</v>
       </c>
       <c r="C68" s="5">
@@ -9586,11 +9598,11 @@
         <v>92526</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="8">
         <v>2</v>
       </c>
       <c r="C69" s="5">
@@ -9603,11 +9615,11 @@
         <v>83169</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="8">
         <v>2</v>
       </c>
       <c r="C70" s="5">
@@ -9620,11 +9632,11 @@
         <v>58190</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="8">
         <v>5</v>
       </c>
       <c r="C71" s="5">
@@ -9637,11 +9649,11 @@
         <v>100503.7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="8">
         <v>5</v>
       </c>
       <c r="C72" s="5">
@@ -9654,11 +9666,11 @@
         <v>86563.4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="8">
         <v>4</v>
       </c>
       <c r="C73" s="5">
@@ -9671,11 +9683,11 @@
         <v>53638</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="8">
         <v>3</v>
       </c>
       <c r="C74" s="5">
@@ -9688,11 +9700,11 @@
         <v>62472</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="8">
         <v>4</v>
       </c>
       <c r="C75" s="5">
@@ -9705,11 +9717,11 @@
         <v>89126</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="8">
         <v>4</v>
       </c>
       <c r="C76" s="5">
@@ -9722,11 +9734,11 @@
         <v>61590</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="8">
         <v>5</v>
       </c>
       <c r="C77" s="5">
@@ -9739,11 +9751,11 @@
         <v>94992.7</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="8">
         <v>2</v>
       </c>
       <c r="C78" s="5">
@@ -9756,11 +9768,11 @@
         <v>40979</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="8">
         <v>5</v>
       </c>
       <c r="C79" s="5">
@@ -9773,11 +9785,11 @@
         <v>99668.800000000003</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="8">
         <v>4</v>
       </c>
       <c r="C80" s="5">
@@ -9790,11 +9802,11 @@
         <v>91632</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="8">
         <v>2</v>
       </c>
       <c r="C81" s="5">
@@ -9807,11 +9819,11 @@
         <v>38413</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="8">
         <v>4</v>
       </c>
       <c r="C82" s="5">
@@ -9824,11 +9836,11 @@
         <v>29892</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="8">
         <v>2</v>
       </c>
       <c r="C83" s="5">
@@ -9841,11 +9853,11 @@
         <v>85414</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="8">
         <v>3</v>
       </c>
       <c r="C84" s="5">
@@ -9858,11 +9870,11 @@
         <v>36220</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="8">
         <v>1</v>
       </c>
       <c r="C85" s="5">
@@ -9875,11 +9887,11 @@
         <v>54102</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="8">
         <v>2</v>
       </c>
       <c r="C86" s="5">
@@ -9892,11 +9904,11 @@
         <v>97719</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="8">
         <v>4</v>
       </c>
       <c r="C87" s="5">
@@ -9909,11 +9921,11 @@
         <v>83237</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="8">
         <v>1</v>
       </c>
       <c r="C88" s="5">
@@ -9926,11 +9938,11 @@
         <v>56934</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="8">
         <v>3</v>
       </c>
       <c r="C89" s="5">
@@ -9943,11 +9955,11 @@
         <v>78859</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="8">
         <v>2</v>
       </c>
       <c r="C90" s="5">
@@ -9960,11 +9972,11 @@
         <v>87369</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="8">
         <v>2</v>
       </c>
       <c r="C91" s="5">
@@ -9977,11 +9989,11 @@
         <v>25504</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="8">
         <v>4</v>
       </c>
       <c r="C92" s="5">
@@ -9994,11 +10006,11 @@
         <v>40689</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="8">
         <v>3</v>
       </c>
       <c r="C93" s="5">
@@ -10011,11 +10023,11 @@
         <v>78844</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="8">
         <v>2</v>
       </c>
       <c r="C94" s="5">
@@ -10028,11 +10040,11 @@
         <v>27077</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="8">
         <v>2</v>
       </c>
       <c r="C95" s="5">
@@ -10045,11 +10057,11 @@
         <v>51225</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="8">
         <v>1</v>
       </c>
       <c r="C96" s="5">
@@ -10062,11 +10074,11 @@
         <v>55175</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="8">
         <v>5</v>
       </c>
       <c r="C97" s="5">
@@ -10079,11 +10091,11 @@
         <v>96295.1</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="8">
         <v>4</v>
       </c>
       <c r="C98" s="5">
@@ -10096,11 +10108,11 @@
         <v>56445</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="8">
         <v>4</v>
       </c>
       <c r="C99" s="5">
@@ -10113,11 +10125,11 @@
         <v>64872</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="8">
         <v>1</v>
       </c>
       <c r="C100" s="5">
@@ -10130,11 +10142,11 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="8">
         <v>4</v>
       </c>
       <c r="C101" s="5">
@@ -10147,11 +10159,11 @@
         <v>48094</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="8">
         <v>5</v>
       </c>
       <c r="C102" s="5">
@@ -10164,11 +10176,11 @@
         <v>43722.8</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B103" s="8">
         <v>287</v>
       </c>
       <c r="C103" s="5">
@@ -10193,89 +10205,89 @@
   </sheetPr>
   <dimension ref="A3:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" customWidth="1"/>
-    <col min="11" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="35" max="40" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="47" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="68" max="72" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="79" max="80" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="91" max="93" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="96" max="104" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="40" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="47" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="72" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="78" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="93" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="104" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>104</v>
       </c>
@@ -10288,193 +10300,193 @@
       <c r="D4" t="s">
         <v>125</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <f>GETPIVOTDATA("Salary",$A$3,"Gender",I$3,"Department",$H4)</f>
         <v>9</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <f>GETPIVOTDATA("Salary",$A$3,"Gender",J$3,"Department",$H4)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>9</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="8">
         <v>9</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="8">
         <v>18</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <f t="shared" ref="I5:J10" si="0">GETPIVOTDATA("Salary",$A$3,"Gender",I$3,"Department",$H5)</f>
         <v>7</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="8">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="8">
         <v>12</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="8">
         <v>9</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="8">
         <v>17</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="8">
         <v>13</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="8">
         <v>3</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="8">
         <v>12</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="8">
         <v>12</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="8">
         <v>6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="8">
         <v>18</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="8">
         <v>7</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="8">
         <v>2</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>62</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="8">
         <v>37</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="8">
         <v>99</v>
       </c>
     </row>

</xml_diff>